<commit_message>
bug fixing ad emissions
</commit_message>
<xml_diff>
--- a/data/forestry.xlsx
+++ b/data/forestry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29728"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuigalwayie-my.sharepoint.com/personal/0121302s_universityofgalway_ie/Documents/03. RESEARCH/01. LIVE PROEJCTS/CAMG Modelling/18. MODEL DEVELOPMENT/INTERFACE/Revisions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C711141F-08BA-4AAE-A645-22AF8FDAF406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA54BE08-A35F-4265-88C1-53E433BD6089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{B86DC117-0B88-41ED-9D24-CA48C208C5B6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{B86DC117-0B88-41ED-9D24-CA48C208C5B6}"/>
   </bookViews>
   <sheets>
     <sheet name="existing_forest" sheetId="1" r:id="rId1"/>
@@ -426,9 +426,6 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -436,6 +433,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -20121,8 +20121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0890E3-5A87-4964-A460-B7480D8C3A7A}">
   <dimension ref="A1:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25923,9 +25923,9 @@
       <c r="O20" s="28">
         <v>0</v>
       </c>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
       <c r="S20" s="23"/>
     </row>
     <row r="21" spans="1:19">
@@ -30088,10 +30088,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8944EF0B-4042-4779-82CE-4B05AD3AA32F}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -30105,10 +30105,10 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>51</v>
       </c>
       <c r="D1" s="13" t="s">
@@ -30169,10 +30169,10 @@
       <c r="A3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -30181,19 +30181,19 @@
       <c r="E3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="33" t="s">
         <v>42</v>
       </c>
     </row>
@@ -30212,8 +30212,8 @@
       <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="20">
-        <v>2025</v>
+      <c r="A5" s="21">
+        <v>2020</v>
       </c>
       <c r="B5" s="23">
         <v>0</v>
@@ -30244,8 +30244,8 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20">
-        <v>2026</v>
+      <c r="A6" s="21">
+        <v>2021</v>
       </c>
       <c r="B6" s="23">
         <v>0</v>
@@ -30276,8 +30276,8 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="20">
-        <v>2027</v>
+      <c r="A7" s="21">
+        <v>2022</v>
       </c>
       <c r="B7" s="23">
         <v>0</v>
@@ -30308,8 +30308,8 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="20">
-        <v>2028</v>
+      <c r="A8" s="21">
+        <v>2023</v>
       </c>
       <c r="B8" s="23">
         <v>0</v>
@@ -30340,8 +30340,8 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="20">
-        <v>2029</v>
+      <c r="A9" s="21">
+        <v>2024</v>
       </c>
       <c r="B9" s="23">
         <v>0</v>
@@ -30373,7 +30373,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="20">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="B10" s="23">
         <v>0</v>
@@ -30405,7 +30405,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="20">
-        <v>2031</v>
+        <v>2026</v>
       </c>
       <c r="B11" s="23">
         <v>0</v>
@@ -30437,7 +30437,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="20">
-        <v>2032</v>
+        <v>2027</v>
       </c>
       <c r="B12" s="23">
         <v>0</v>
@@ -30469,7 +30469,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="20">
-        <v>2033</v>
+        <v>2028</v>
       </c>
       <c r="B13" s="23">
         <v>0</v>
@@ -30501,7 +30501,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="20">
-        <v>2034</v>
+        <v>2029</v>
       </c>
       <c r="B14" s="23">
         <v>0</v>
@@ -30533,38 +30533,31 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="20">
-        <v>2035</v>
-      </c>
-      <c r="B15" s="28">
-        <f>((C15*1000*16)/3600)*0.85</f>
-        <v>419.371839293123</v>
-      </c>
-      <c r="C15" s="28">
-        <f>D15*8.8</f>
-        <v>111.01019275406196</v>
-      </c>
-      <c r="D15" s="28">
-        <f>D20/6</f>
-        <v>12.614794631143404</v>
-      </c>
-      <c r="E15" s="28">
-        <f>D15</f>
-        <v>12.614794631143404</v>
-      </c>
-      <c r="F15" s="28">
-        <f>-(((((8.8/2)*1.5)-2)*3.67)/20)*D15</f>
-        <v>-10.648148148148149</v>
-      </c>
-      <c r="G15" s="30">
-        <f>-B15*0.255*0.1</f>
-        <v>-10.693981901974638</v>
+        <v>2030</v>
+      </c>
+      <c r="B15" s="23">
+        <v>0</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
+      <c r="D15" s="23">
+        <v>0</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
+      <c r="F15" s="23">
+        <v>0</v>
+      </c>
+      <c r="G15" s="23">
+        <v>0</v>
       </c>
       <c r="H15" s="23">
         <v>0</v>
       </c>
-      <c r="I15" s="28">
-        <f>I20/6</f>
-        <v>166.66666666666666</v>
+      <c r="I15" s="23">
+        <v>0</v>
       </c>
       <c r="J15" s="23">
         <v>0</v>
@@ -30572,38 +30565,31 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="20">
-        <v>2036</v>
-      </c>
-      <c r="B16" s="28">
-        <f t="shared" ref="B16:B79" si="0">((C16*1000*16)/3600)*0.85</f>
-        <v>838.74367858624601</v>
-      </c>
-      <c r="C16" s="28">
-        <f t="shared" ref="C16:C79" si="1">D16*8.8</f>
-        <v>222.02038550812392</v>
-      </c>
-      <c r="D16" s="28">
-        <f>D15+(D$20/6)</f>
-        <v>25.229589262286808</v>
-      </c>
-      <c r="E16" s="28">
-        <f t="shared" ref="E16:E19" si="2">D16</f>
-        <v>25.229589262286808</v>
-      </c>
-      <c r="F16" s="28">
-        <f t="shared" ref="F16:F39" si="3">-(((((8.8/2)*1.5)-2)*3.67)/20)*D16</f>
-        <v>-21.296296296296298</v>
-      </c>
-      <c r="G16" s="30">
-        <f t="shared" ref="G16:G79" si="4">-B16*0.255*0.1</f>
-        <v>-21.387963803949276</v>
+        <v>2031</v>
+      </c>
+      <c r="B16" s="23">
+        <v>0</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0</v>
+      </c>
+      <c r="F16" s="23">
+        <v>0</v>
+      </c>
+      <c r="G16" s="23">
+        <v>0</v>
       </c>
       <c r="H16" s="23">
         <v>0</v>
       </c>
-      <c r="I16" s="28">
-        <f>I15+(I$20/6)</f>
-        <v>333.33333333333331</v>
+      <c r="I16" s="23">
+        <v>0</v>
       </c>
       <c r="J16" s="23">
         <v>0</v>
@@ -30611,314 +30597,298 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="20">
+        <v>2032</v>
+      </c>
+      <c r="B17" s="23">
+        <v>0</v>
+      </c>
+      <c r="C17" s="23">
+        <v>0</v>
+      </c>
+      <c r="D17" s="23">
+        <v>0</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0</v>
+      </c>
+      <c r="G17" s="23">
+        <v>0</v>
+      </c>
+      <c r="H17" s="23">
+        <v>0</v>
+      </c>
+      <c r="I17" s="23">
+        <v>0</v>
+      </c>
+      <c r="J17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="20">
+        <v>2033</v>
+      </c>
+      <c r="B18" s="23">
+        <v>0</v>
+      </c>
+      <c r="C18" s="23">
+        <v>0</v>
+      </c>
+      <c r="D18" s="23">
+        <v>0</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0</v>
+      </c>
+      <c r="F18" s="23">
+        <v>0</v>
+      </c>
+      <c r="G18" s="23">
+        <v>0</v>
+      </c>
+      <c r="H18" s="23">
+        <v>0</v>
+      </c>
+      <c r="I18" s="23">
+        <v>0</v>
+      </c>
+      <c r="J18" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="20">
+        <v>2034</v>
+      </c>
+      <c r="B19" s="23">
+        <v>0</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0</v>
+      </c>
+      <c r="D19" s="23">
+        <v>0</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0</v>
+      </c>
+      <c r="F19" s="23">
+        <v>0</v>
+      </c>
+      <c r="G19" s="23">
+        <v>0</v>
+      </c>
+      <c r="H19" s="23">
+        <v>0</v>
+      </c>
+      <c r="I19" s="23">
+        <v>0</v>
+      </c>
+      <c r="J19" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="20">
+        <v>2035</v>
+      </c>
+      <c r="B20" s="28">
+        <f>((C20*1000*16)/3600)*0.85</f>
+        <v>419.371839293123</v>
+      </c>
+      <c r="C20" s="28">
+        <f>D20*8.8</f>
+        <v>111.01019275406196</v>
+      </c>
+      <c r="D20" s="28">
+        <f>D25/6</f>
+        <v>12.614794631143404</v>
+      </c>
+      <c r="E20" s="28">
+        <f>D20</f>
+        <v>12.614794631143404</v>
+      </c>
+      <c r="F20" s="28">
+        <f>-(((((8.8/2)*1.5)-2)*3.67)/20)*D20</f>
+        <v>-10.648148148148149</v>
+      </c>
+      <c r="G20" s="30">
+        <f>-B20*0.255*0.1</f>
+        <v>-10.693981901974638</v>
+      </c>
+      <c r="H20" s="23">
+        <v>0</v>
+      </c>
+      <c r="I20" s="28">
+        <f>I25/6</f>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="J20" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="20">
+        <v>2036</v>
+      </c>
+      <c r="B21" s="28">
+        <f t="shared" ref="B21:B84" si="0">((C21*1000*16)/3600)*0.85</f>
+        <v>838.74367858624601</v>
+      </c>
+      <c r="C21" s="28">
+        <f t="shared" ref="C21:C84" si="1">D21*8.8</f>
+        <v>222.02038550812392</v>
+      </c>
+      <c r="D21" s="28">
+        <f>D20+(D$25/6)</f>
+        <v>25.229589262286808</v>
+      </c>
+      <c r="E21" s="28">
+        <f t="shared" ref="E21:E24" si="2">D21</f>
+        <v>25.229589262286808</v>
+      </c>
+      <c r="F21" s="28">
+        <f t="shared" ref="F21:F44" si="3">-(((((8.8/2)*1.5)-2)*3.67)/20)*D21</f>
+        <v>-21.296296296296298</v>
+      </c>
+      <c r="G21" s="30">
+        <f t="shared" ref="G21:G84" si="4">-B21*0.255*0.1</f>
+        <v>-21.387963803949276</v>
+      </c>
+      <c r="H21" s="23">
+        <v>0</v>
+      </c>
+      <c r="I21" s="28">
+        <f>I20+(I$25/6)</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="J21" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="20">
         <v>2037</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B22" s="28">
         <f t="shared" si="0"/>
         <v>1258.115517879369</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C22" s="28">
         <f t="shared" si="1"/>
         <v>333.03057826218588</v>
       </c>
-      <c r="D17" s="28">
-        <f>D16+(D$20/6)</f>
+      <c r="D22" s="28">
+        <f>D21+(D$25/6)</f>
         <v>37.844383893430212</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E22" s="28">
         <f t="shared" si="2"/>
         <v>37.844383893430212</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F22" s="28">
         <f t="shared" si="3"/>
         <v>-31.944444444444446</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G22" s="30">
         <f t="shared" si="4"/>
         <v>-32.081945705923907</v>
       </c>
-      <c r="H17" s="23">
-        <v>0</v>
-      </c>
-      <c r="I17" s="28">
-        <f t="shared" ref="I17:I19" si="5">I16+(I$20/6)</f>
+      <c r="H22" s="23">
+        <v>0</v>
+      </c>
+      <c r="I22" s="28">
+        <f t="shared" ref="I22:I24" si="5">I21+(I$25/6)</f>
         <v>500</v>
       </c>
-      <c r="J17" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="20">
+      <c r="J22" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="20">
         <v>2038</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B23" s="28">
         <f t="shared" si="0"/>
         <v>1677.487357172492</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C23" s="28">
         <f t="shared" si="1"/>
         <v>444.04077101624785</v>
       </c>
-      <c r="D18" s="28">
-        <f>D17+(D$20/6)</f>
+      <c r="D23" s="28">
+        <f>D22+(D$25/6)</f>
         <v>50.459178524573616</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E23" s="28">
         <f t="shared" si="2"/>
         <v>50.459178524573616</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F23" s="28">
         <f t="shared" si="3"/>
         <v>-42.592592592592595</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G23" s="30">
         <f t="shared" si="4"/>
         <v>-42.775927607898552</v>
       </c>
-      <c r="H18" s="23">
-        <v>0</v>
-      </c>
-      <c r="I18" s="28">
+      <c r="H23" s="23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="28">
         <f t="shared" si="5"/>
         <v>666.66666666666663</v>
       </c>
-      <c r="J18" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="20">
+      <c r="J23" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="20">
         <v>2039</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B24" s="28">
         <f t="shared" si="0"/>
         <v>2096.8591964656148</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C24" s="28">
         <f t="shared" si="1"/>
         <v>555.05096377030986</v>
       </c>
-      <c r="D19" s="28">
-        <f>D18+(D$20/6)</f>
+      <c r="D24" s="28">
+        <f>D23+(D$25/6)</f>
         <v>63.07397315571702</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E24" s="28">
         <f t="shared" si="2"/>
         <v>63.07397315571702</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F24" s="28">
         <f t="shared" si="3"/>
         <v>-53.24074074074074</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G24" s="30">
         <f t="shared" si="4"/>
         <v>-53.469909509873176</v>
       </c>
-      <c r="H19" s="23">
-        <v>0</v>
-      </c>
-      <c r="I19" s="28">
+      <c r="H24" s="23">
+        <v>0</v>
+      </c>
+      <c r="I24" s="28">
         <f t="shared" si="5"/>
         <v>833.33333333333326</v>
       </c>
-      <c r="J19" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="20">
-        <v>2040</v>
-      </c>
-      <c r="B20" s="28">
-        <f t="shared" si="0"/>
-        <v>2516.231035758738</v>
-      </c>
-      <c r="C20" s="28">
-        <f t="shared" si="1"/>
-        <v>666.06115652437177</v>
-      </c>
-      <c r="D20" s="28">
-        <f>((((I20/0.9)/3.67)*2))/8</f>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="E20" s="28">
-        <f>D20</f>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="F20" s="28">
-        <f t="shared" si="3"/>
-        <v>-63.888888888888893</v>
-      </c>
-      <c r="G20" s="30">
-        <f t="shared" si="4"/>
-        <v>-64.163891411847814</v>
-      </c>
-      <c r="H20" s="23">
-        <v>0</v>
-      </c>
-      <c r="I20" s="28">
-        <v>1000</v>
-      </c>
-      <c r="J20" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="20">
-        <v>2041</v>
-      </c>
-      <c r="B21" s="28">
-        <f t="shared" si="0"/>
-        <v>2516.231035758738</v>
-      </c>
-      <c r="C21" s="28">
-        <f t="shared" si="1"/>
-        <v>666.06115652437177</v>
-      </c>
-      <c r="D21" s="28">
-        <f>D20</f>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="E21" s="28">
-        <f>E20</f>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="F21" s="28">
-        <f t="shared" si="3"/>
-        <v>-63.888888888888893</v>
-      </c>
-      <c r="G21" s="30">
-        <f t="shared" si="4"/>
-        <v>-64.163891411847814</v>
-      </c>
-      <c r="H21" s="23">
-        <v>0</v>
-      </c>
-      <c r="I21" s="28">
-        <v>1000</v>
-      </c>
-      <c r="J21" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="20">
-        <v>2042</v>
-      </c>
-      <c r="B22" s="28">
-        <f t="shared" si="0"/>
-        <v>2516.231035758738</v>
-      </c>
-      <c r="C22" s="28">
-        <f t="shared" si="1"/>
-        <v>666.06115652437177</v>
-      </c>
-      <c r="D22" s="28">
-        <f t="shared" ref="D22:E37" si="6">D21</f>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="E22" s="28">
-        <f t="shared" si="6"/>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="F22" s="28">
-        <f t="shared" si="3"/>
-        <v>-63.888888888888893</v>
-      </c>
-      <c r="G22" s="30">
-        <f t="shared" si="4"/>
-        <v>-64.163891411847814</v>
-      </c>
-      <c r="H22" s="23">
-        <v>0</v>
-      </c>
-      <c r="I22" s="28">
-        <v>1000</v>
-      </c>
-      <c r="J22" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="20">
-        <v>2043</v>
-      </c>
-      <c r="B23" s="28">
-        <f t="shared" si="0"/>
-        <v>2516.231035758738</v>
-      </c>
-      <c r="C23" s="28">
-        <f t="shared" si="1"/>
-        <v>666.06115652437177</v>
-      </c>
-      <c r="D23" s="28">
-        <f t="shared" si="6"/>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="E23" s="28">
-        <f t="shared" si="6"/>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="F23" s="28">
-        <f t="shared" si="3"/>
-        <v>-63.888888888888893</v>
-      </c>
-      <c r="G23" s="30">
-        <f t="shared" si="4"/>
-        <v>-64.163891411847814</v>
-      </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="28">
-        <v>1000</v>
-      </c>
-      <c r="J23" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="20">
-        <v>2044</v>
-      </c>
-      <c r="B24" s="28">
-        <f t="shared" si="0"/>
-        <v>2516.231035758738</v>
-      </c>
-      <c r="C24" s="28">
-        <f t="shared" si="1"/>
-        <v>666.06115652437177</v>
-      </c>
-      <c r="D24" s="28">
-        <f t="shared" si="6"/>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="E24" s="28">
-        <f t="shared" si="6"/>
-        <v>75.688767786860424</v>
-      </c>
-      <c r="F24" s="28">
-        <f t="shared" si="3"/>
-        <v>-63.888888888888893</v>
-      </c>
-      <c r="G24" s="30">
-        <f t="shared" si="4"/>
-        <v>-64.163891411847814</v>
-      </c>
-      <c r="H24" s="23">
-        <v>0</v>
-      </c>
-      <c r="I24" s="28">
-        <v>1000</v>
-      </c>
       <c r="J24" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="20">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B25" s="28">
         <f t="shared" si="0"/>
@@ -30929,11 +30899,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D25" s="28">
-        <f t="shared" si="6"/>
+        <f>((((I25/0.9)/3.67)*2))/8</f>
         <v>75.688767786860424</v>
       </c>
       <c r="E25" s="28">
-        <f t="shared" si="6"/>
+        <f>D25</f>
         <v>75.688767786860424</v>
       </c>
       <c r="F25" s="28">
@@ -30956,7 +30926,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="20">
-        <v>2046</v>
+        <v>2041</v>
       </c>
       <c r="B26" s="28">
         <f t="shared" si="0"/>
@@ -30967,11 +30937,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D26" s="28">
-        <f t="shared" si="6"/>
+        <f>D25</f>
         <v>75.688767786860424</v>
       </c>
       <c r="E26" s="28">
-        <f t="shared" si="6"/>
+        <f>E25</f>
         <v>75.688767786860424</v>
       </c>
       <c r="F26" s="28">
@@ -30994,7 +30964,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="20">
-        <v>2047</v>
+        <v>2042</v>
       </c>
       <c r="B27" s="28">
         <f t="shared" si="0"/>
@@ -31005,7 +30975,7 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D27" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D27:E42" si="6">D26</f>
         <v>75.688767786860424</v>
       </c>
       <c r="E27" s="28">
@@ -31032,7 +31002,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="20">
-        <v>2048</v>
+        <v>2043</v>
       </c>
       <c r="B28" s="28">
         <f t="shared" si="0"/>
@@ -31070,7 +31040,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="20">
-        <v>2049</v>
+        <v>2044</v>
       </c>
       <c r="B29" s="28">
         <f t="shared" si="0"/>
@@ -31108,7 +31078,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="20">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="B30" s="28">
         <f t="shared" si="0"/>
@@ -31146,7 +31116,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="20">
-        <v>2051</v>
+        <v>2046</v>
       </c>
       <c r="B31" s="28">
         <f t="shared" si="0"/>
@@ -31184,7 +31154,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="20">
-        <v>2052</v>
+        <v>2047</v>
       </c>
       <c r="B32" s="28">
         <f t="shared" si="0"/>
@@ -31222,7 +31192,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="20">
-        <v>2053</v>
+        <v>2048</v>
       </c>
       <c r="B33" s="28">
         <f t="shared" si="0"/>
@@ -31260,7 +31230,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="20">
-        <v>2054</v>
+        <v>2049</v>
       </c>
       <c r="B34" s="28">
         <f t="shared" si="0"/>
@@ -31298,7 +31268,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="20">
-        <v>2055</v>
+        <v>2050</v>
       </c>
       <c r="B35" s="28">
         <f t="shared" si="0"/>
@@ -31336,7 +31306,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="20">
-        <v>2056</v>
+        <v>2051</v>
       </c>
       <c r="B36" s="28">
         <f t="shared" si="0"/>
@@ -31374,7 +31344,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="20">
-        <v>2057</v>
+        <v>2052</v>
       </c>
       <c r="B37" s="28">
         <f t="shared" si="0"/>
@@ -31412,7 +31382,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="20">
-        <v>2058</v>
+        <v>2053</v>
       </c>
       <c r="B38" s="28">
         <f t="shared" si="0"/>
@@ -31423,11 +31393,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D38" s="28">
-        <f t="shared" ref="D38:E53" si="7">D37</f>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E38" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F38" s="28">
@@ -31450,7 +31420,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="20">
-        <v>2059</v>
+        <v>2054</v>
       </c>
       <c r="B39" s="28">
         <f t="shared" si="0"/>
@@ -31461,11 +31431,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D39" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E39" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F39" s="28">
@@ -31488,7 +31458,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="20">
-        <v>2060</v>
+        <v>2055</v>
       </c>
       <c r="B40" s="28">
         <f t="shared" si="0"/>
@@ -31499,15 +31469,16 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D40" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E40" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F40" s="28">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-63.888888888888893</v>
       </c>
       <c r="G40" s="30">
         <f t="shared" si="4"/>
@@ -31525,7 +31496,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="20">
-        <v>2061</v>
+        <v>2056</v>
       </c>
       <c r="B41" s="28">
         <f t="shared" si="0"/>
@@ -31536,15 +31507,16 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D41" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E41" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F41" s="28">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-63.888888888888893</v>
       </c>
       <c r="G41" s="30">
         <f t="shared" si="4"/>
@@ -31562,7 +31534,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="20">
-        <v>2062</v>
+        <v>2057</v>
       </c>
       <c r="B42" s="28">
         <f t="shared" si="0"/>
@@ -31573,15 +31545,16 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D42" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E42" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F42" s="28">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-63.888888888888893</v>
       </c>
       <c r="G42" s="30">
         <f t="shared" si="4"/>
@@ -31599,7 +31572,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="20">
-        <v>2063</v>
+        <v>2058</v>
       </c>
       <c r="B43" s="28">
         <f t="shared" si="0"/>
@@ -31610,7 +31583,7 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D43" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="D43:E58" si="7">D42</f>
         <v>75.688767786860424</v>
       </c>
       <c r="E43" s="28">
@@ -31618,7 +31591,8 @@
         <v>75.688767786860424</v>
       </c>
       <c r="F43" s="28">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-63.888888888888893</v>
       </c>
       <c r="G43" s="30">
         <f t="shared" si="4"/>
@@ -31636,7 +31610,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="20">
-        <v>2064</v>
+        <v>2059</v>
       </c>
       <c r="B44" s="28">
         <f t="shared" si="0"/>
@@ -31655,7 +31629,8 @@
         <v>75.688767786860424</v>
       </c>
       <c r="F44" s="28">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-63.888888888888893</v>
       </c>
       <c r="G44" s="30">
         <f t="shared" si="4"/>
@@ -31673,7 +31648,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="20">
-        <v>2065</v>
+        <v>2060</v>
       </c>
       <c r="B45" s="28">
         <f t="shared" si="0"/>
@@ -31710,7 +31685,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="20">
-        <v>2066</v>
+        <v>2061</v>
       </c>
       <c r="B46" s="28">
         <f t="shared" si="0"/>
@@ -31747,7 +31722,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="20">
-        <v>2067</v>
+        <v>2062</v>
       </c>
       <c r="B47" s="28">
         <f t="shared" si="0"/>
@@ -31784,7 +31759,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="20">
-        <v>2068</v>
+        <v>2063</v>
       </c>
       <c r="B48" s="28">
         <f t="shared" si="0"/>
@@ -31821,7 +31796,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="20">
-        <v>2069</v>
+        <v>2064</v>
       </c>
       <c r="B49" s="28">
         <f t="shared" si="0"/>
@@ -31858,7 +31833,7 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="20">
-        <v>2070</v>
+        <v>2065</v>
       </c>
       <c r="B50" s="28">
         <f t="shared" si="0"/>
@@ -31895,7 +31870,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="20">
-        <v>2071</v>
+        <v>2066</v>
       </c>
       <c r="B51" s="28">
         <f t="shared" si="0"/>
@@ -31932,7 +31907,7 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="20">
-        <v>2072</v>
+        <v>2067</v>
       </c>
       <c r="B52" s="28">
         <f t="shared" si="0"/>
@@ -31969,7 +31944,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="20">
-        <v>2073</v>
+        <v>2068</v>
       </c>
       <c r="B53" s="28">
         <f t="shared" si="0"/>
@@ -32006,7 +31981,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="20">
-        <v>2074</v>
+        <v>2069</v>
       </c>
       <c r="B54" s="28">
         <f t="shared" si="0"/>
@@ -32017,11 +31992,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D54" s="28">
-        <f t="shared" ref="D54:E69" si="8">D53</f>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E54" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F54" s="28">
@@ -32043,7 +32018,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="20">
-        <v>2075</v>
+        <v>2070</v>
       </c>
       <c r="B55" s="28">
         <f t="shared" si="0"/>
@@ -32054,11 +32029,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D55" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E55" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F55" s="28">
@@ -32080,7 +32055,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="20">
-        <v>2076</v>
+        <v>2071</v>
       </c>
       <c r="B56" s="28">
         <f t="shared" si="0"/>
@@ -32091,11 +32066,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D56" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E56" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F56" s="28">
@@ -32117,7 +32092,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="20">
-        <v>2077</v>
+        <v>2072</v>
       </c>
       <c r="B57" s="28">
         <f t="shared" si="0"/>
@@ -32128,11 +32103,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D57" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E57" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F57" s="28">
@@ -32154,7 +32129,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="20">
-        <v>2078</v>
+        <v>2073</v>
       </c>
       <c r="B58" s="28">
         <f t="shared" si="0"/>
@@ -32165,11 +32140,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D58" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E58" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F58" s="28">
@@ -32191,7 +32166,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="20">
-        <v>2079</v>
+        <v>2074</v>
       </c>
       <c r="B59" s="28">
         <f t="shared" si="0"/>
@@ -32202,7 +32177,7 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D59" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="D59:E74" si="8">D58</f>
         <v>75.688767786860424</v>
       </c>
       <c r="E59" s="28">
@@ -32228,7 +32203,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="20">
-        <v>2080</v>
+        <v>2075</v>
       </c>
       <c r="B60" s="28">
         <f t="shared" si="0"/>
@@ -32265,7 +32240,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="20">
-        <v>2081</v>
+        <v>2076</v>
       </c>
       <c r="B61" s="28">
         <f t="shared" si="0"/>
@@ -32302,7 +32277,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="20">
-        <v>2082</v>
+        <v>2077</v>
       </c>
       <c r="B62" s="28">
         <f t="shared" si="0"/>
@@ -32339,7 +32314,7 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="20">
-        <v>2083</v>
+        <v>2078</v>
       </c>
       <c r="B63" s="28">
         <f t="shared" si="0"/>
@@ -32376,7 +32351,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="20">
-        <v>2084</v>
+        <v>2079</v>
       </c>
       <c r="B64" s="28">
         <f t="shared" si="0"/>
@@ -32413,7 +32388,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="20">
-        <v>2085</v>
+        <v>2080</v>
       </c>
       <c r="B65" s="28">
         <f t="shared" si="0"/>
@@ -32450,7 +32425,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="20">
-        <v>2086</v>
+        <v>2081</v>
       </c>
       <c r="B66" s="28">
         <f t="shared" si="0"/>
@@ -32487,7 +32462,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="20">
-        <v>2087</v>
+        <v>2082</v>
       </c>
       <c r="B67" s="28">
         <f t="shared" si="0"/>
@@ -32524,7 +32499,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="20">
-        <v>2088</v>
+        <v>2083</v>
       </c>
       <c r="B68" s="28">
         <f t="shared" si="0"/>
@@ -32561,7 +32536,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="20">
-        <v>2089</v>
+        <v>2084</v>
       </c>
       <c r="B69" s="28">
         <f t="shared" si="0"/>
@@ -32598,7 +32573,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="20">
-        <v>2090</v>
+        <v>2085</v>
       </c>
       <c r="B70" s="28">
         <f t="shared" si="0"/>
@@ -32609,11 +32584,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D70" s="28">
-        <f t="shared" ref="D70:E80" si="9">D69</f>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E70" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F70" s="28">
@@ -32635,7 +32610,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="20">
-        <v>2091</v>
+        <v>2086</v>
       </c>
       <c r="B71" s="28">
         <f t="shared" si="0"/>
@@ -32646,11 +32621,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D71" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E71" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F71" s="28">
@@ -32672,7 +32647,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="20">
-        <v>2092</v>
+        <v>2087</v>
       </c>
       <c r="B72" s="28">
         <f t="shared" si="0"/>
@@ -32683,11 +32658,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D72" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E72" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F72" s="28">
@@ -32709,7 +32684,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="20">
-        <v>2093</v>
+        <v>2088</v>
       </c>
       <c r="B73" s="28">
         <f t="shared" si="0"/>
@@ -32720,11 +32695,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D73" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E73" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F73" s="28">
@@ -32746,7 +32721,7 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="20">
-        <v>2094</v>
+        <v>2089</v>
       </c>
       <c r="B74" s="28">
         <f t="shared" si="0"/>
@@ -32757,11 +32732,11 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D74" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="E74" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>75.688767786860424</v>
       </c>
       <c r="F74" s="28">
@@ -32783,7 +32758,7 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="20">
-        <v>2095</v>
+        <v>2090</v>
       </c>
       <c r="B75" s="28">
         <f t="shared" si="0"/>
@@ -32794,7 +32769,7 @@
         <v>666.06115652437177</v>
       </c>
       <c r="D75" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="D75:E85" si="9">D74</f>
         <v>75.688767786860424</v>
       </c>
       <c r="E75" s="28">
@@ -32820,7 +32795,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="20">
-        <v>2096</v>
+        <v>2091</v>
       </c>
       <c r="B76" s="28">
         <f t="shared" si="0"/>
@@ -32857,7 +32832,7 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="20">
-        <v>2097</v>
+        <v>2092</v>
       </c>
       <c r="B77" s="28">
         <f t="shared" si="0"/>
@@ -32894,7 +32869,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="20">
-        <v>2098</v>
+        <v>2093</v>
       </c>
       <c r="B78" s="28">
         <f t="shared" si="0"/>
@@ -32931,7 +32906,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="20">
-        <v>2099</v>
+        <v>2094</v>
       </c>
       <c r="B79" s="28">
         <f t="shared" si="0"/>
@@ -32968,14 +32943,14 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="20">
-        <v>2100</v>
+        <v>2095</v>
       </c>
       <c r="B80" s="28">
-        <f t="shared" ref="B80" si="10">((C80*1000*16)/3600)*0.85</f>
+        <f t="shared" si="0"/>
         <v>2516.231035758738</v>
       </c>
       <c r="C80" s="28">
-        <f t="shared" ref="C80" si="11">D80*8.8</f>
+        <f t="shared" si="1"/>
         <v>666.06115652437177</v>
       </c>
       <c r="D80" s="28">
@@ -32990,7 +32965,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="30">
-        <f t="shared" ref="G80" si="12">-B80*0.255*0.1</f>
+        <f t="shared" si="4"/>
         <v>-64.163891411847814</v>
       </c>
       <c r="H80" s="23">
@@ -33004,16 +32979,201 @@
       </c>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="20"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="26"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="23"/>
-      <c r="J81" s="23"/>
+      <c r="A81" s="20">
+        <v>2096</v>
+      </c>
+      <c r="B81" s="28">
+        <f t="shared" si="0"/>
+        <v>2516.231035758738</v>
+      </c>
+      <c r="C81" s="28">
+        <f t="shared" si="1"/>
+        <v>666.06115652437177</v>
+      </c>
+      <c r="D81" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="E81" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="F81" s="28">
+        <v>0</v>
+      </c>
+      <c r="G81" s="30">
+        <f t="shared" si="4"/>
+        <v>-64.163891411847814</v>
+      </c>
+      <c r="H81" s="23">
+        <v>0</v>
+      </c>
+      <c r="I81" s="28">
+        <v>1000</v>
+      </c>
+      <c r="J81" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="20">
+        <v>2097</v>
+      </c>
+      <c r="B82" s="28">
+        <f t="shared" si="0"/>
+        <v>2516.231035758738</v>
+      </c>
+      <c r="C82" s="28">
+        <f t="shared" si="1"/>
+        <v>666.06115652437177</v>
+      </c>
+      <c r="D82" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="E82" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="F82" s="28">
+        <v>0</v>
+      </c>
+      <c r="G82" s="30">
+        <f t="shared" si="4"/>
+        <v>-64.163891411847814</v>
+      </c>
+      <c r="H82" s="23">
+        <v>0</v>
+      </c>
+      <c r="I82" s="28">
+        <v>1000</v>
+      </c>
+      <c r="J82" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="20">
+        <v>2098</v>
+      </c>
+      <c r="B83" s="28">
+        <f t="shared" si="0"/>
+        <v>2516.231035758738</v>
+      </c>
+      <c r="C83" s="28">
+        <f t="shared" si="1"/>
+        <v>666.06115652437177</v>
+      </c>
+      <c r="D83" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="E83" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="F83" s="28">
+        <v>0</v>
+      </c>
+      <c r="G83" s="30">
+        <f t="shared" si="4"/>
+        <v>-64.163891411847814</v>
+      </c>
+      <c r="H83" s="23">
+        <v>0</v>
+      </c>
+      <c r="I83" s="28">
+        <v>1000</v>
+      </c>
+      <c r="J83" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="20">
+        <v>2099</v>
+      </c>
+      <c r="B84" s="28">
+        <f t="shared" si="0"/>
+        <v>2516.231035758738</v>
+      </c>
+      <c r="C84" s="28">
+        <f t="shared" si="1"/>
+        <v>666.06115652437177</v>
+      </c>
+      <c r="D84" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="E84" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="F84" s="28">
+        <v>0</v>
+      </c>
+      <c r="G84" s="30">
+        <f t="shared" si="4"/>
+        <v>-64.163891411847814</v>
+      </c>
+      <c r="H84" s="23">
+        <v>0</v>
+      </c>
+      <c r="I84" s="28">
+        <v>1000</v>
+      </c>
+      <c r="J84" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="20">
+        <v>2100</v>
+      </c>
+      <c r="B85" s="28">
+        <f t="shared" ref="B85" si="10">((C85*1000*16)/3600)*0.85</f>
+        <v>2516.231035758738</v>
+      </c>
+      <c r="C85" s="28">
+        <f t="shared" ref="C85" si="11">D85*8.8</f>
+        <v>666.06115652437177</v>
+      </c>
+      <c r="D85" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="E85" s="28">
+        <f t="shared" si="9"/>
+        <v>75.688767786860424</v>
+      </c>
+      <c r="F85" s="28">
+        <v>0</v>
+      </c>
+      <c r="G85" s="30">
+        <f t="shared" ref="G85" si="12">-B85*0.255*0.1</f>
+        <v>-64.163891411847814</v>
+      </c>
+      <c r="H85" s="23">
+        <v>0</v>
+      </c>
+      <c r="I85" s="28">
+        <v>1000</v>
+      </c>
+      <c r="J85" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="20"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="23"/>
+      <c r="J86" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>